<commit_message>
updated with dhmo1 expression data
updated dHMO1 expression data and altered the labels so they weren't capitalized; i.e. dCIN5 --> dcin5
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/16-genes_36-edges_NW-wt-fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/16-genes_36-edges_NW-wt-fam_Sigmoid_estimation.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14025" tabRatio="500" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14025" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="4" r:id="rId1"/>
     <sheet name="degradation_rates" sheetId="3" r:id="rId2"/>
     <sheet name="wt_log2_expression" sheetId="5" r:id="rId3"/>
-    <sheet name="dCIN5_log2_expression" sheetId="7" r:id="rId4"/>
-    <sheet name="dGLN3_log2_expression" sheetId="8" r:id="rId5"/>
-    <sheet name="dHAP4_log2_expression" sheetId="9" r:id="rId6"/>
-    <sheet name="dZAP1_log2_expression" sheetId="10" r:id="rId7"/>
-    <sheet name="network" sheetId="1" r:id="rId8"/>
-    <sheet name="network_weights" sheetId="2" r:id="rId9"/>
-    <sheet name="optimization_parameters" sheetId="6" r:id="rId10"/>
-    <sheet name="threshold_b" sheetId="11" r:id="rId11"/>
+    <sheet name="dcin5_log2_expression" sheetId="7" r:id="rId4"/>
+    <sheet name="dgln3_log2_expression" sheetId="8" r:id="rId5"/>
+    <sheet name="dhap4_log2_expression" sheetId="9" r:id="rId6"/>
+    <sheet name="dhmo1_log2_expression" sheetId="12" r:id="rId7"/>
+    <sheet name="dzap1_log2_expression" sheetId="10" r:id="rId8"/>
+    <sheet name="network" sheetId="1" r:id="rId9"/>
+    <sheet name="network_weights" sheetId="2" r:id="rId10"/>
+    <sheet name="optimization_parameters" sheetId="6" r:id="rId11"/>
+    <sheet name="threshold_b" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
   <si>
     <t>ABF1</t>
   </si>
@@ -156,9 +157,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -256,161 +264,163 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="132" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="132" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="132" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="132" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="133"/>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="134">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -544,6 +554,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Normal 3" xfId="132"/>
+    <cellStyle name="Normal 4" xfId="133"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1037,6 +1048,927 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1229,11 +2161,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2342,7 +3274,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="A1:XFD1048576"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3062,8 +3994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3801,7 +4733,7 @@
     <sortCondition ref="B18:B33"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3815,7 +4747,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="A1:M17"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4532,6 +5464,718 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="17">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17">
+        <v>15</v>
+      </c>
+      <c r="D1" s="17">
+        <v>15</v>
+      </c>
+      <c r="E1" s="17">
+        <v>15</v>
+      </c>
+      <c r="F1" s="17">
+        <v>30</v>
+      </c>
+      <c r="G1" s="17">
+        <v>30</v>
+      </c>
+      <c r="H1" s="17">
+        <v>30</v>
+      </c>
+      <c r="I1" s="17">
+        <v>30</v>
+      </c>
+      <c r="J1" s="17">
+        <v>60</v>
+      </c>
+      <c r="K1" s="17">
+        <v>60</v>
+      </c>
+      <c r="L1" s="17">
+        <v>60</v>
+      </c>
+      <c r="M1" s="17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17">
+        <v>-0.93340000000000001</v>
+      </c>
+      <c r="C2" s="17">
+        <v>-0.49109999999999998</v>
+      </c>
+      <c r="D2" s="17">
+        <v>-1.0347</v>
+      </c>
+      <c r="E2" s="17">
+        <v>-5.4300000000000001E-2</v>
+      </c>
+      <c r="F2" s="17">
+        <v>-2.8940000000000001</v>
+      </c>
+      <c r="G2" s="17">
+        <v>-0.88290000000000002</v>
+      </c>
+      <c r="H2" s="17">
+        <v>-0.53500000000000003</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0.129</v>
+      </c>
+      <c r="J2" s="17">
+        <v>-2.5434000000000001</v>
+      </c>
+      <c r="K2" s="17">
+        <v>-1.8429</v>
+      </c>
+      <c r="L2" s="17">
+        <v>0.9224</v>
+      </c>
+      <c r="M2" s="17">
+        <v>-0.4647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <v>0.2392</v>
+      </c>
+      <c r="C3" s="17">
+        <v>-0.3695</v>
+      </c>
+      <c r="D3" s="17">
+        <v>-1.0907</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.17549999999999999</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="G3" s="17">
+        <v>-0.19889999999999999</v>
+      </c>
+      <c r="H3" s="17">
+        <v>-0.95930000000000004</v>
+      </c>
+      <c r="I3" s="17">
+        <v>-0.2329</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="K3" s="17">
+        <v>-0.49980000000000002</v>
+      </c>
+      <c r="L3" s="17">
+        <v>-0.29909999999999998</v>
+      </c>
+      <c r="M3" s="17">
+        <v>-0.23880000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.71870000000000001</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1.6315</v>
+      </c>
+      <c r="D4" s="17">
+        <v>3.2448000000000001</v>
+      </c>
+      <c r="E4" s="17">
+        <v>-3.2275</v>
+      </c>
+      <c r="F4" s="17">
+        <v>-2.3641000000000001</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0.9244</v>
+      </c>
+      <c r="I4" s="17">
+        <v>-2.6962999999999999</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0.31990000000000002</v>
+      </c>
+      <c r="K4" s="17">
+        <v>2.9540999999999999</v>
+      </c>
+      <c r="L4" s="17">
+        <v>-0.8337</v>
+      </c>
+      <c r="M4" s="17">
+        <v>-2.5552000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="C5" s="17">
+        <v>-0.10440000000000001</v>
+      </c>
+      <c r="D5" s="17">
+        <v>7.6E-3</v>
+      </c>
+      <c r="E5" s="17">
+        <v>-0.97260000000000002</v>
+      </c>
+      <c r="F5" s="17">
+        <v>-8.8400000000000006E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <v>-1.1843999999999999</v>
+      </c>
+      <c r="H5" s="17">
+        <v>-0.51300000000000001</v>
+      </c>
+      <c r="I5" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J5" s="17">
+        <v>-1.7664</v>
+      </c>
+      <c r="K5" s="17">
+        <v>-2.3744000000000001</v>
+      </c>
+      <c r="L5" s="17">
+        <v>-0.42449999999999999</v>
+      </c>
+      <c r="M5" s="17">
+        <v>-0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1.0969</v>
+      </c>
+      <c r="D6" s="17">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="E6" s="17">
+        <v>-0.43659999999999999</v>
+      </c>
+      <c r="F6" s="17">
+        <v>-2.2907000000000002</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.50260000000000005</v>
+      </c>
+      <c r="H6" s="17">
+        <v>-0.27150000000000002</v>
+      </c>
+      <c r="I6" s="17">
+        <v>-0.57410000000000005</v>
+      </c>
+      <c r="J6" s="17">
+        <v>-1.5159</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1.7901</v>
+      </c>
+      <c r="M6" s="17">
+        <v>-0.87539999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0.62390000000000001</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.81840000000000002</v>
+      </c>
+      <c r="D7" s="17">
+        <v>1.4916</v>
+      </c>
+      <c r="E7" s="17">
+        <v>-0.8397</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.88670000000000004</v>
+      </c>
+      <c r="G7" s="17">
+        <v>1.2386999999999999</v>
+      </c>
+      <c r="H7" s="17">
+        <v>2.2606000000000002</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0.32929999999999998</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1.2067000000000001</v>
+      </c>
+      <c r="K7" s="17">
+        <v>1.7983</v>
+      </c>
+      <c r="L7" s="17">
+        <v>-0.70660000000000001</v>
+      </c>
+      <c r="M7" s="17">
+        <v>1.0147999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1.1274999999999999</v>
+      </c>
+      <c r="C8" s="17">
+        <v>-0.15479999999999999</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="E8" s="17">
+        <v>-1.8301000000000001</v>
+      </c>
+      <c r="F8" s="17">
+        <v>-0.82740000000000002</v>
+      </c>
+      <c r="G8" s="17">
+        <v>-8.3599999999999994E-2</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0.62150000000000005</v>
+      </c>
+      <c r="I8" s="17">
+        <v>-0.80579999999999996</v>
+      </c>
+      <c r="J8" s="17">
+        <v>0.55489999999999995</v>
+      </c>
+      <c r="K8" s="17">
+        <v>-0.25569999999999998</v>
+      </c>
+      <c r="L8" s="17">
+        <v>-1.5242</v>
+      </c>
+      <c r="M8" s="17">
+        <v>-1.1165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17">
+        <v>-0.39379999999999998</v>
+      </c>
+      <c r="C9" s="17">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="D9" s="17">
+        <v>-0.97989999999999999</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="F9" s="17">
+        <v>-0.56820000000000004</v>
+      </c>
+      <c r="G9" s="17">
+        <v>-7.2800000000000004E-2</v>
+      </c>
+      <c r="H9" s="17">
+        <v>-0.186</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0.63060000000000005</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0.29170000000000001</v>
+      </c>
+      <c r="K9" s="17">
+        <v>-0.1706</v>
+      </c>
+      <c r="L9" s="17">
+        <v>0.29249999999999998</v>
+      </c>
+      <c r="M9" s="17">
+        <v>0.89139999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17">
+        <v>0.2944</v>
+      </c>
+      <c r="C10" s="17">
+        <v>-1.0325</v>
+      </c>
+      <c r="D10" s="17">
+        <v>-0.34420000000000001</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.89370000000000005</v>
+      </c>
+      <c r="F10" s="17">
+        <v>-1.5780000000000001</v>
+      </c>
+      <c r="G10" s="17">
+        <v>-1.4498</v>
+      </c>
+      <c r="H10" s="17">
+        <v>-0.73839999999999995</v>
+      </c>
+      <c r="I10" s="17">
+        <v>-0.2666</v>
+      </c>
+      <c r="J10" s="17">
+        <v>-1.5417000000000001</v>
+      </c>
+      <c r="K10" s="17">
+        <v>-3.0545</v>
+      </c>
+      <c r="L10" s="17">
+        <v>1.8973</v>
+      </c>
+      <c r="M10" s="17">
+        <v>-0.88439999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1.0058</v>
+      </c>
+      <c r="C11" s="17">
+        <v>-3.1699999999999999E-2</v>
+      </c>
+      <c r="D11" s="17">
+        <v>2.0181</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.78879999999999995</v>
+      </c>
+      <c r="F11" s="17">
+        <v>-0.20660000000000001</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.3846</v>
+      </c>
+      <c r="H11" s="17">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0.1787</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0.1767</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0.48980000000000001</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0.83540000000000003</v>
+      </c>
+      <c r="M11" s="17">
+        <v>0.46439999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-0.32290000000000002</v>
+      </c>
+      <c r="C12" s="17">
+        <v>-0.37169999999999997</v>
+      </c>
+      <c r="D12" s="17">
+        <v>-0.80130000000000001</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.4516</v>
+      </c>
+      <c r="F12" s="17">
+        <v>-0.37780000000000002</v>
+      </c>
+      <c r="G12" s="17">
+        <v>-0.32479999999999998</v>
+      </c>
+      <c r="H12" s="17">
+        <v>-0.47610000000000002</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0.95050000000000001</v>
+      </c>
+      <c r="J12" s="17">
+        <v>-0.2303</v>
+      </c>
+      <c r="K12" s="17">
+        <v>-0.56030000000000002</v>
+      </c>
+      <c r="L12" s="17">
+        <v>1.2226999999999999</v>
+      </c>
+      <c r="M12" s="17">
+        <v>0.57889999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1.2329000000000001</v>
+      </c>
+      <c r="C13" s="17">
+        <v>2.2441</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.49480000000000002</v>
+      </c>
+      <c r="E13" s="17">
+        <v>-0.69450000000000001</v>
+      </c>
+      <c r="F13" s="17">
+        <v>-0.83460000000000001</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1.8561000000000001</v>
+      </c>
+      <c r="H13" s="17">
+        <v>-0.52869999999999995</v>
+      </c>
+      <c r="I13" s="17">
+        <v>-0.60660000000000003</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1.3966000000000001</v>
+      </c>
+      <c r="L13" s="17">
+        <v>-0.15140000000000001</v>
+      </c>
+      <c r="M13" s="17">
+        <v>-0.58509999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17">
+        <v>0.52490000000000003</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0.1762</v>
+      </c>
+      <c r="D14" s="17">
+        <v>-0.16950000000000001</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.33610000000000001</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1.0117</v>
+      </c>
+      <c r="G14" s="17">
+        <v>-0.54710000000000003</v>
+      </c>
+      <c r="H14" s="17">
+        <v>-0.14910000000000001</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0.26079999999999998</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0.74080000000000001</v>
+      </c>
+      <c r="K14" s="17">
+        <v>-0.57830000000000004</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0.45569999999999999</v>
+      </c>
+      <c r="M14" s="17">
+        <v>0.52290000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17">
+        <v>-0.182</v>
+      </c>
+      <c r="C15" s="17">
+        <v>-1.0702</v>
+      </c>
+      <c r="D15" s="17">
+        <v>-0.84470000000000001</v>
+      </c>
+      <c r="E15" s="17">
+        <v>-1.0067999999999999</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.1177</v>
+      </c>
+      <c r="G15" s="17">
+        <v>-0.35110000000000002</v>
+      </c>
+      <c r="H15" s="17">
+        <v>2.24E-2</v>
+      </c>
+      <c r="I15" s="17">
+        <v>-0.61650000000000005</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="K15" s="17">
+        <v>-1.1442000000000001</v>
+      </c>
+      <c r="L15" s="17">
+        <v>-0.80579999999999996</v>
+      </c>
+      <c r="M15" s="17">
+        <v>0.14030000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="17">
+        <v>-2.4929000000000001</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-0.45329999999999998</v>
+      </c>
+      <c r="D16" s="17">
+        <v>-0.22650000000000001</v>
+      </c>
+      <c r="E16" s="17">
+        <v>-1.1136999999999999</v>
+      </c>
+      <c r="F16" s="17">
+        <v>-0.91169999999999995</v>
+      </c>
+      <c r="G16" s="17">
+        <v>-0.248</v>
+      </c>
+      <c r="H16" s="17">
+        <v>-7.8299999999999995E-2</v>
+      </c>
+      <c r="I16" s="17">
+        <v>-1.7543</v>
+      </c>
+      <c r="J16" s="17">
+        <v>-0.77810000000000001</v>
+      </c>
+      <c r="K16" s="17">
+        <v>-0.3231</v>
+      </c>
+      <c r="L16" s="17">
+        <v>0.2596</v>
+      </c>
+      <c r="M16" s="17">
+        <v>-2.0924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="17">
+        <v>-0.23080000000000001</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-0.39169999999999999</v>
+      </c>
+      <c r="D17" s="17">
+        <v>-1.0017</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.17660000000000001</v>
+      </c>
+      <c r="F17" s="17">
+        <v>1.17E-2</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0.17510000000000001</v>
+      </c>
+      <c r="H17" s="17">
+        <v>-0.97560000000000002</v>
+      </c>
+      <c r="I17" s="17">
+        <v>-0.53039999999999998</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0.44109999999999999</v>
+      </c>
+      <c r="K17" s="17">
+        <v>-0.70899999999999996</v>
+      </c>
+      <c r="L17" s="17">
+        <v>-9.9000000000000008E-3</v>
+      </c>
+      <c r="M17" s="17">
+        <v>0.84150000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="A1:M17"/>
     </sheetView>
@@ -5233,928 +6877,6 @@
       </c>
       <c r="M17" s="2">
         <v>-0.8246</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:Q17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>1</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6180,7 +6902,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -7081,6 +7803,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
changed convention for network
altered A1 cell to have "targets" rather than "affected"
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/16-genes_36-edges_NW-wt-fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/16-genes_36-edges_NW-wt-fam_Sigmoid_estimation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwilli31\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14025" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5550" tabRatio="500" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="4" r:id="rId1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="40">
   <si>
     <t>ABF1</t>
   </si>
@@ -82,12 +87,6 @@
   </si>
   <si>
     <t>degradation_rate</t>
-  </si>
-  <si>
-    <t>cols regulators/rows affected</t>
-  </si>
-  <si>
-    <t>cols regulating/rows affected</t>
   </si>
   <si>
     <t>alpha</t>
@@ -149,6 +148,9 @@
   <si>
     <t>wt</t>
   </si>
+  <si>
+    <t>cols regulators/rows targets</t>
+  </si>
 </sst>
 </file>
 
@@ -206,15 +208,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -561,6 +566,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1050,15 +1058,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1982,15 +1990,15 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>2E-3</v>
@@ -1998,7 +2006,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -2006,7 +2014,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>100000000</v>
@@ -2014,7 +2022,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3">
         <v>9.9999999999999995E-7</v>
@@ -2022,7 +2030,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3">
         <v>100000000</v>
@@ -2030,7 +2038,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>9.9999999999999995E-7</v>
@@ -2038,15 +2046,15 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2054,7 +2062,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -2062,7 +2070,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
@@ -2070,7 +2078,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -2078,7 +2086,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -2086,7 +2094,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2">
         <v>15</v>
@@ -2100,15 +2108,15 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -2179,7 +2187,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2324,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6894,15 +6902,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:Q17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>

</xml_diff>